<commit_message>
update: documentos atualizado e finalizados
</commit_message>
<xml_diff>
--- a/Docs/Product-Backlog-Meowmory.xlsx
+++ b/Docs/Product-Backlog-Meowmory.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E136D00F-C0CB-4950-933E-0E55A015B261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramir\OneDrive\Documentos\Project-Meowmory\Docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD4D925E-1738-44D1-911A-E47CE22AEE8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PRODUCT-BACKLOG" sheetId="1" r:id="rId1"/>
@@ -32,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="113">
   <si>
     <t>PRODUCT BACKLOG - MEOWMORY</t>
   </si>
@@ -362,13 +367,22 @@
   </si>
   <si>
     <t>Garantir que o sistema se adapte a diferente tamanho de monitores.</t>
+  </si>
+  <si>
+    <t>RNF</t>
+  </si>
+  <si>
+    <t>Estrelinhas no site</t>
+  </si>
+  <si>
+    <t>Adicionar um mural com estrelinhas com base na quantidade de gatos homenageados na plataforma</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -413,6 +427,21 @@
       <color theme="0"/>
       <name val="Grandview"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Grandview Display"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Grandview Display"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -629,7 +658,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -670,74 +699,32 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -749,6 +736,45 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -758,10 +784,94 @@
   <dxfs count="30">
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <name val="Grandview Display"/>
       </font>
       <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial Nova"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -789,7 +899,7 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -809,7 +919,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -837,7 +947,78 @@
     </dxf>
     <dxf>
       <font>
+        <name val="Grandview Display"/>
+      </font>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Grandview Display"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Grandview Display"/>
+      </font>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Grandview Display"/>
+      </font>
+      <alignment horizontal="left" vertical="center" relativeIndent="1"/>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
+        <name val="Grandview Display"/>
+      </font>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <name val="Grandview Display"/>
+      </font>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <name val="Grandview Display"/>
+      </font>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <name val="Grandview Display"/>
+      </font>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <name val="Grandview Display"/>
+      </font>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -857,108 +1038,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Grandview Display"/>
-      </font>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="medium">
-          <color rgb="FF000000"/>
-        </right>
-        <bottom style="medium">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Grandview Display"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Grandview Display"/>
-      </font>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Grandview Display"/>
-      </font>
-      <alignment horizontal="left" vertical="center" relativeIndent="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <name val="Grandview Display"/>
-      </font>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <name val="Grandview Display"/>
-      </font>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <name val="Grandview Display"/>
-      </font>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <name val="Grandview Display"/>
-      </font>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <name val="Grandview Display"/>
-      </font>
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -986,7 +1066,7 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -1006,7 +1086,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1034,33 +1114,14 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial Nova"/>
-        <scheme val="none"/>
+        <name val="Grandview Display"/>
       </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center"/>
     </dxf>
     <dxf>
       <font>
         <name val="Grandview Display"/>
       </font>
-      <alignment horizontal="center" vertical="center"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -1079,11 +1140,6 @@
       <font>
         <name val="Grandview Display"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Grandview Display"/>
-      </font>
       <alignment vertical="center"/>
     </dxf>
     <dxf>
@@ -1091,36 +1147,6 @@
         <name val="Grandview Display"/>
       </font>
       <alignment horizontal="left" vertical="center" relativeIndent="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -1140,9 +1166,13 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E10E1BDB-D26B-4DE3-AF4D-CE07FCA7273B}" name="Tabela4" displayName="Tabela4" ref="B3:I33" headerRowDxfId="26" dataDxfId="25" totalsRowDxfId="24" tableBorderDxfId="23">
-  <autoFilter ref="B3:I33" xr:uid="{E10E1BDB-D26B-4DE3-AF4D-CE07FCA7273B}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E10E1BDB-D26B-4DE3-AF4D-CE07FCA7273B}" name="Tabela4" displayName="Tabela4" ref="B3:I34" headerRowDxfId="29" dataDxfId="28" totalsRowDxfId="26" tableBorderDxfId="27">
+  <autoFilter ref="B3:I34" xr:uid="{E10E1BDB-D26B-4DE3-AF4D-CE07FCA7273B}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -1153,23 +1183,23 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{2AD1D804-0CBC-4A32-BD1B-0A87F0717708}" name="ID" totalsRowLabel="Total" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{5D7CEC9E-8C92-42D6-8D9E-BFB809CFECC8}" name="REQUISITOS" dataDxfId="20" totalsRowDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{9E62E117-2240-4F25-A84D-8A03EF52188C}" name="DESCRIÇÃO" dataDxfId="18" totalsRowDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{71D8F69E-8E0E-4D87-A9DE-BC173F5A8AF2}" name="CLASSIFICAÇÃO" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{F7B48FC9-1238-4573-ABC5-7ABBF7A8D2D4}" name="TAMANHO" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{34BA276E-2F98-431C-B157-4C5AC6D48565}" name="TAM(#)" dataDxfId="15">
+    <tableColumn id="1" xr3:uid="{2AD1D804-0CBC-4A32-BD1B-0A87F0717708}" name="ID" totalsRowLabel="Total" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{5D7CEC9E-8C92-42D6-8D9E-BFB809CFECC8}" name="REQUISITOS" dataDxfId="24" totalsRowDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{9E62E117-2240-4F25-A84D-8A03EF52188C}" name="DESCRIÇÃO" dataDxfId="22" totalsRowDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{71D8F69E-8E0E-4D87-A9DE-BC173F5A8AF2}" name="CLASSIFICAÇÃO" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{F7B48FC9-1238-4573-ABC5-7ABBF7A8D2D4}" name="TAMANHO" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{34BA276E-2F98-431C-B157-4C5AC6D48565}" name="TAM(#)" dataDxfId="18">
       <calculatedColumnFormula>IF(F4="M", 8, IF(F4="G", 13, IF(F4="P", 5, "")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{D484C123-5179-4AE3-BE2B-218ECF8CEAC6}" name="PRIORIDADE" dataDxfId="14"/>
-    <tableColumn id="8" xr3:uid="{114D59C1-EC37-47B3-A16F-78A587D5FA94}" name="SEMANA" totalsRowFunction="count" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{D484C123-5179-4AE3-BE2B-218ECF8CEAC6}" name="PRIORIDADE" dataDxfId="17"/>
+    <tableColumn id="8" xr3:uid="{114D59C1-EC37-47B3-A16F-78A587D5FA94}" name="SEMANA" totalsRowFunction="count" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65998304-2356-4E55-B8AB-A9C40CE03C53}" name="Tabela42" displayName="Tabela42" ref="B3:E33" headerRowDxfId="9" dataDxfId="8" totalsRowDxfId="7" tableBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65998304-2356-4E55-B8AB-A9C40CE03C53}" name="Tabela42" displayName="Tabela42" ref="B3:E33" headerRowDxfId="15" dataDxfId="14" totalsRowDxfId="12" tableBorderDxfId="13">
   <autoFilter ref="B3:E33" xr:uid="{65998304-2356-4E55-B8AB-A9C40CE03C53}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1177,10 +1207,10 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{4294B917-1D65-44A7-A0DA-C9C3E5C62EA9}" name="ID" totalsRowLabel="Total" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{90747139-D216-4938-A6FB-36079796041B}" name="REQUISITOS" dataDxfId="3" totalsRowDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{2B9932F0-1D4D-4707-9695-937E382947DA}" name="DESCRIÇÃO" dataDxfId="1" totalsRowDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{653C62BB-E58B-4AAE-8EDE-9C58CC0A5F73}" name="CLASSIFICAÇÃO" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{4294B917-1D65-44A7-A0DA-C9C3E5C62EA9}" name="ID" totalsRowLabel="Total" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{90747139-D216-4938-A6FB-36079796041B}" name="REQUISITOS" dataDxfId="10" totalsRowDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{2B9932F0-1D4D-4707-9695-937E382947DA}" name="DESCRIÇÃO" dataDxfId="8" totalsRowDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{653C62BB-E58B-4AAE-8EDE-9C58CC0A5F73}" name="CLASSIFICAÇÃO" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1508,37 +1538,37 @@
   </sheetPr>
   <dimension ref="B2:M34"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:I33"/>
+    <sheetView tabSelected="1" zoomScale="77" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="3" max="3" width="41.140625" customWidth="1"/>
-    <col min="4" max="4" width="75.5703125" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.7109375" style="18" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" customWidth="1"/>
+    <col min="3" max="3" width="41.109375" customWidth="1"/>
+    <col min="4" max="4" width="75.5546875" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" style="9" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" style="9" customWidth="1"/>
+    <col min="12" max="12" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.6640625" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" ht="24.75" customHeight="1">
-      <c r="B2" s="14" t="s">
+    <row r="2" spans="2:13" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="16"/>
-    </row>
-    <row r="3" spans="2:13" ht="23.25" customHeight="1">
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="34"/>
+    </row>
+    <row r="3" spans="2:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1564,7 +1594,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:13" ht="45" customHeight="1">
+    <row r="4" spans="2:13" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
@@ -1590,12 +1620,12 @@
       <c r="I4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="L4" s="19" t="s">
+      <c r="L4" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="M4" s="20"/>
-    </row>
-    <row r="5" spans="2:13" ht="45" customHeight="1">
+      <c r="M4" s="36"/>
+    </row>
+    <row r="5" spans="2:13" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>16</v>
       </c>
@@ -1606,7 +1636,7 @@
         <v>18</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>20</v>
@@ -1621,15 +1651,15 @@
       <c r="I5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="L5" s="21" t="s">
+      <c r="L5" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="M5" s="23">
-        <f>SUM(G4:G33)</f>
+      <c r="M5" s="27">
+        <f>SUM(G4:G34)</f>
         <v>246</v>
       </c>
     </row>
-    <row r="6" spans="2:13" ht="45" customHeight="1">
+    <row r="6" spans="2:13" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>22</v>
       </c>
@@ -1655,15 +1685,15 @@
       <c r="I6" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="L6" s="22" t="s">
+      <c r="L6" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="M6" s="24">
-        <f>SUMIF(I4:I33,"SEMANA - 1", G4:G33)</f>
+      <c r="M6" s="28">
+        <f>SUMIF(I4:I34,"SEMANA - 1", G4:G34)</f>
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="2:13" ht="45" customHeight="1">
+    <row r="7" spans="2:13" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>26</v>
       </c>
@@ -1673,7 +1703,7 @@
       <c r="D7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="30" t="s">
         <v>12</v>
       </c>
       <c r="F7" s="11" t="s">
@@ -1689,15 +1719,15 @@
       <c r="I7" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="L7" s="22" t="s">
+      <c r="L7" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="M7" s="24">
-        <f>SUMIF(I4:I33,"SEMANA - 2", G4:G33)</f>
+      <c r="M7" s="28">
+        <f>SUMIF(I4:I34,"SEMANA - 2", G4:G34)</f>
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="2:13" ht="45" customHeight="1">
+    <row r="8" spans="2:13" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>30</v>
       </c>
@@ -1707,7 +1737,7 @@
       <c r="D8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="30" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="11" t="s">
@@ -1723,15 +1753,15 @@
       <c r="I8" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="L8" s="22" t="s">
+      <c r="L8" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="M8" s="24">
-        <f>SUMIF(I4:I33,"SEMANA - 3", G4:G33)</f>
+      <c r="M8" s="28">
+        <f>SUMIF(I4:I34,"SEMANA - 3", G4:G34)</f>
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="2:13" ht="45" customHeight="1">
+    <row r="9" spans="2:13" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>33</v>
       </c>
@@ -1741,7 +1771,7 @@
       <c r="D9" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="29" t="s">
         <v>19</v>
       </c>
       <c r="F9" s="11" t="s">
@@ -1757,15 +1787,15 @@
       <c r="I9" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="L9" s="22" t="s">
+      <c r="L9" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="M9" s="24">
-        <f>SUMIF(I4:I33,"SEMANA - 4", G4:G33)</f>
+      <c r="M9" s="28">
+        <f>SUMIF(I4:I34,"SEMANA - 4", G4:G34)</f>
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="2:13" ht="45" customHeight="1">
+    <row r="10" spans="2:13" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>37</v>
       </c>
@@ -1775,8 +1805,8 @@
       <c r="D10" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="11" t="s">
-        <v>12</v>
+      <c r="E10" s="30" t="s">
+        <v>67</v>
       </c>
       <c r="F10" s="11" t="s">
         <v>13</v>
@@ -1791,15 +1821,15 @@
       <c r="I10" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="L10" s="21" t="s">
+      <c r="L10" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="M10" s="25">
+      <c r="M10" s="18">
         <f>M5/4</f>
         <v>61.5</v>
       </c>
     </row>
-    <row r="11" spans="2:13" ht="45" customHeight="1">
+    <row r="11" spans="2:13" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>41</v>
       </c>
@@ -1809,8 +1839,8 @@
       <c r="D11" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="11" t="s">
-        <v>12</v>
+      <c r="E11" s="30" t="s">
+        <v>67</v>
       </c>
       <c r="F11" s="11" t="s">
         <v>13</v>
@@ -1826,7 +1856,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="2:13" ht="45" customHeight="1">
+    <row r="12" spans="2:13" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
         <v>44</v>
       </c>
@@ -1853,7 +1883,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="2:13" ht="45" customHeight="1">
+    <row r="13" spans="2:13" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>48</v>
       </c>
@@ -1880,7 +1910,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="2:13" ht="45" customHeight="1">
+    <row r="14" spans="2:13" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>51</v>
       </c>
@@ -1907,7 +1937,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="2:13" ht="45" customHeight="1">
+    <row r="15" spans="2:13" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
         <v>54</v>
       </c>
@@ -1934,7 +1964,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="2:13" ht="45" customHeight="1">
+    <row r="16" spans="2:13" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
         <v>58</v>
       </c>
@@ -1961,7 +1991,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="2:9" ht="45" customHeight="1">
+    <row r="17" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>61</v>
       </c>
@@ -1988,7 +2018,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="2:9" ht="45" customHeight="1">
+    <row r="18" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
         <v>64</v>
       </c>
@@ -2015,7 +2045,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="2:9" ht="45" customHeight="1">
+    <row r="19" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>68</v>
       </c>
@@ -2042,7 +2072,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="2:9" ht="45" customHeight="1">
+    <row r="20" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
         <v>71</v>
       </c>
@@ -2069,7 +2099,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="2:9" ht="45" customHeight="1">
+    <row r="21" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
         <v>74</v>
       </c>
@@ -2096,7 +2126,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="2:9" ht="45" customHeight="1">
+    <row r="22" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
         <v>77</v>
       </c>
@@ -2123,7 +2153,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="2:9" ht="45" customHeight="1">
+    <row r="23" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
         <v>80</v>
       </c>
@@ -2150,20 +2180,20 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="2:9" ht="26.25" customHeight="1">
+    <row r="24" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="6"/>
       <c r="C24" s="7"/>
       <c r="D24" s="8"/>
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
-      <c r="G24" s="17" t="str">
+      <c r="G24" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H24" s="12"/>
       <c r="I24" s="12"/>
     </row>
-    <row r="25" spans="2:9" ht="45" customHeight="1">
+    <row r="25" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
         <v>83</v>
       </c>
@@ -2190,7 +2220,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="2:9" ht="45" customHeight="1">
+    <row r="26" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
         <v>86</v>
       </c>
@@ -2217,7 +2247,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="2:9" ht="45" customHeight="1">
+    <row r="27" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="2" t="s">
         <v>89</v>
       </c>
@@ -2244,7 +2274,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="2:9" ht="45" customHeight="1">
+    <row r="28" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="2" t="s">
         <v>92</v>
       </c>
@@ -2271,7 +2301,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="2:9" ht="45" customHeight="1">
+    <row r="29" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="2" t="s">
         <v>95</v>
       </c>
@@ -2298,7 +2328,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="2:9" ht="45" customHeight="1">
+    <row r="30" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="2" t="s">
         <v>98</v>
       </c>
@@ -2325,7 +2355,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="2:9" ht="45" customHeight="1">
+    <row r="31" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="2" t="s">
         <v>101</v>
       </c>
@@ -2352,7 +2382,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="2:9" ht="45" customHeight="1">
+    <row r="32" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="2" t="s">
         <v>104</v>
       </c>
@@ -2379,7 +2409,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="2:9" ht="45" customHeight="1">
+    <row r="33" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="2" t="s">
         <v>107</v>
       </c>
@@ -2406,25 +2436,41 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="2:9" ht="45" customHeight="1"/>
+    <row r="34" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11" t="str">
+        <f>IF(F34="M", 8, IF(F34="G", 13, IF(F34="P", 5, "")))</f>
+        <v/>
+      </c>
+      <c r="H34" s="11"/>
+      <c r="I34" s="11"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="L4:M4"/>
   </mergeCells>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="29" priority="3" stopIfTrue="1" operator="equal">
-      <formula>"Essencial"</formula>
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+      <formula>"Desejável"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="28" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"Importante"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="27" priority="1" operator="equal">
-      <formula>"Desejável"</formula>
+    <cfRule type="cellIs" dxfId="3" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"Essencial"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2442,327 +2488,327 @@
   </sheetPr>
   <dimension ref="B2:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E24"/>
+    <sheetView zoomScale="91" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="45" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="45" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="42" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="77.85546875" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" customWidth="1"/>
+    <col min="4" max="4" width="77.88671875" customWidth="1"/>
+    <col min="5" max="5" width="23.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="45" customHeight="1">
-      <c r="B2" s="26" t="s">
+    <row r="2" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="28"/>
-    </row>
-    <row r="3" spans="2:5" ht="45" customHeight="1">
-      <c r="B3" s="29" t="s">
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="39"/>
+    </row>
+    <row r="3" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="31" t="s">
+      <c r="E3" s="20" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="45" customHeight="1">
-      <c r="B4" s="32" t="s">
+    <row r="4" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="35" t="s">
+      <c r="E4" s="22" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="45" customHeight="1">
-      <c r="B5" s="32" t="s">
+    <row r="5" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="31" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="22" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="45" customHeight="1">
-      <c r="B6" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="35" t="s">
+    <row r="10" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="31" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="22" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="45" customHeight="1">
-      <c r="B7" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="33" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="35" t="s">
+    <row r="13" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="22" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="2:5" ht="45" customHeight="1">
-      <c r="B8" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="35" t="s">
+    <row r="14" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="22" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="2:5" ht="45" customHeight="1">
-      <c r="B9" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" s="35" t="s">
+    <row r="15" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="22" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="45" customHeight="1">
-      <c r="B10" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" s="35" t="s">
+    <row r="16" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="22" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="45" customHeight="1">
-      <c r="B11" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="E11" s="35" t="s">
+    <row r="17" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" s="22" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E22" s="22" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="2:5" ht="45" customHeight="1">
-      <c r="B12" s="32" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" s="35" t="s">
+    <row r="23" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E23" s="22" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="2:5" ht="45" customHeight="1">
-      <c r="B13" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" s="34" t="s">
-        <v>50</v>
-      </c>
-      <c r="E13" s="35" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" ht="45" customHeight="1">
-      <c r="B14" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="D14" s="34" t="s">
-        <v>53</v>
-      </c>
-      <c r="E14" s="35" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" ht="45" customHeight="1">
-      <c r="B15" s="32" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" s="36" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" s="35" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" ht="45" customHeight="1">
-      <c r="B16" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="C16" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="D16" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="E16" s="35" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" ht="45" customHeight="1">
-      <c r="B17" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" s="33" t="s">
-        <v>62</v>
-      </c>
-      <c r="D17" s="34" t="s">
-        <v>63</v>
-      </c>
-      <c r="E17" s="35" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" ht="45" customHeight="1">
-      <c r="B18" s="32" t="s">
-        <v>64</v>
-      </c>
-      <c r="C18" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="D18" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="E18" s="35" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" ht="45" customHeight="1">
-      <c r="B19" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="C19" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="D19" s="34" t="s">
-        <v>70</v>
-      </c>
-      <c r="E19" s="35" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" ht="45" customHeight="1">
-      <c r="B20" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="C20" s="36" t="s">
-        <v>72</v>
-      </c>
-      <c r="D20" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="E20" s="35" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" ht="45" customHeight="1">
-      <c r="B21" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="C21" s="33" t="s">
-        <v>75</v>
-      </c>
-      <c r="D21" s="34" t="s">
-        <v>76</v>
-      </c>
-      <c r="E21" s="35" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" ht="45" customHeight="1">
-      <c r="B22" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="C22" s="33" t="s">
-        <v>78</v>
-      </c>
-      <c r="D22" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="E22" s="35" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" ht="45" customHeight="1">
-      <c r="B23" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="C23" s="33" t="s">
-        <v>81</v>
-      </c>
-      <c r="D23" s="34" t="s">
-        <v>82</v>
-      </c>
-      <c r="E23" s="35" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" ht="45" customHeight="1">
-      <c r="B24" s="37"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="39"/>
-      <c r="E24" s="40"/>
-    </row>
-    <row r="25" spans="2:5" ht="45" customHeight="1">
+    <row r="24" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="23"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="26"/>
+    </row>
+    <row r="25" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
         <v>83</v>
       </c>
@@ -2776,7 +2822,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="2:5" ht="45" customHeight="1">
+    <row r="26" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
         <v>86</v>
       </c>
@@ -2790,7 +2836,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="2:5" ht="45" customHeight="1">
+    <row r="27" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="2" t="s">
         <v>89</v>
       </c>
@@ -2804,7 +2850,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="2:5" ht="45" customHeight="1">
+    <row r="28" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="2" t="s">
         <v>92</v>
       </c>
@@ -2818,7 +2864,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="2:5" ht="45" customHeight="1">
+    <row r="29" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="2" t="s">
         <v>95</v>
       </c>
@@ -2832,7 +2878,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="2:5" ht="45" customHeight="1">
+    <row r="30" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="2" t="s">
         <v>98</v>
       </c>
@@ -2846,7 +2892,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="2:5" ht="45" customHeight="1">
+    <row r="31" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="2" t="s">
         <v>101</v>
       </c>
@@ -2860,7 +2906,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="2:5" ht="45" customHeight="1">
+    <row r="32" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="2" t="s">
         <v>104</v>
       </c>
@@ -2874,7 +2920,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="33" spans="2:5" ht="45" customHeight="1">
+    <row r="33" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="2" t="s">
         <v>107</v>
       </c>
@@ -2893,24 +2939,20 @@
     <mergeCell ref="B2:E2"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:E33">
-    <cfRule type="cellIs" dxfId="12" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"Desejável"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"Importante"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" stopIfTrue="1" operator="equal">
       <formula>"Essencial"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E33">
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
-      <formula>"Importante"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E33">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
-      <formula>"Desejável"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" scale="46" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>